<commit_message>
feat: Creación de KPI's
</commit_message>
<xml_diff>
--- a/Dashboard/Dashboard.xlsx
+++ b/Dashboard/Dashboard.xlsx
@@ -5,28 +5,32 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\servicios_cul_soci_depor_recre\data\processed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\servicios_cul_soci_depor_recre\Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F61F8FE8-1CB3-4881-851A-0D81324AD972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{15019FF8-4902-4F16-BE4D-33FA2BC777E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" activeTab="1" xr2:uid="{0F6DE12B-782F-43E4-BCEE-D62EF1718F31}"/>
+    <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" activeTab="5" xr2:uid="{0F6DE12B-782F-43E4-BCEE-D62EF1718F31}"/>
   </bookViews>
   <sheets>
     <sheet name="servicios_cult_soc_dep_rec_isss" sheetId="1" r:id="rId1"/>
     <sheet name="Servios deportivos por año" sheetId="2" r:id="rId2"/>
     <sheet name="Comp entre cul vs dep vs soc" sheetId="3" r:id="rId3"/>
     <sheet name="Ranking de delegaciones" sheetId="4" r:id="rId4"/>
+    <sheet name="Ranking de Servicios" sheetId="6" r:id="rId5"/>
+    <sheet name="KPI's" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="21" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="5" r:id="rId8"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="85">
   <si>
     <t>Aguascalientes</t>
   </si>
@@ -263,6 +267,24 @@
   </si>
   <si>
     <t>Ranking de oficinas de representación</t>
+  </si>
+  <si>
+    <t>Etiquetas de fila</t>
+  </si>
+  <si>
+    <t>Suma de Suma de todos los Servicios</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Nombre Servicio</t>
+  </si>
+  <si>
+    <t>Total de cada servicio</t>
+  </si>
+  <si>
+    <t>Suma de Total de cada servicio</t>
   </si>
 </sst>
 </file>
@@ -818,7 +840,13 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -879,7 +907,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Dashboard.xlsx]Servios deportivos por año!ServiciosDeportivosPorAño</c:name>
+    <c:name>[Dashboard(Recuperado automáticamente).xlsx]Servios deportivos por año!ServiciosDeportivosPorAño</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -918,6 +946,9 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -984,6 +1015,9 @@
       <c:pivotFmt>
         <c:idx val="1"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1050,6 +1084,9 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1116,6 +1153,9 @@
       <c:pivotFmt>
         <c:idx val="3"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1182,6 +1222,9 @@
       <c:pivotFmt>
         <c:idx val="4"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1248,6 +1291,9 @@
       <c:pivotFmt>
         <c:idx val="5"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1314,6 +1360,9 @@
       <c:pivotFmt>
         <c:idx val="6"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1380,6 +1429,9 @@
       <c:pivotFmt>
         <c:idx val="7"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1446,6 +1498,9 @@
       <c:pivotFmt>
         <c:idx val="8"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1512,6 +1567,9 @@
       <c:pivotFmt>
         <c:idx val="9"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1578,6 +1636,9 @@
       <c:pivotFmt>
         <c:idx val="10"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1644,6 +1705,9 @@
       <c:pivotFmt>
         <c:idx val="11"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1710,6 +1774,9 @@
       <c:pivotFmt>
         <c:idx val="12"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1776,6 +1843,9 @@
       <c:pivotFmt>
         <c:idx val="13"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1842,6 +1912,9 @@
       <c:pivotFmt>
         <c:idx val="14"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1908,6 +1981,9 @@
       <c:pivotFmt>
         <c:idx val="15"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1974,6 +2050,9 @@
       <c:pivotFmt>
         <c:idx val="16"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2040,6 +2119,9 @@
       <c:pivotFmt>
         <c:idx val="17"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2106,6 +2188,9 @@
       <c:pivotFmt>
         <c:idx val="18"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2172,6 +2257,9 @@
       <c:pivotFmt>
         <c:idx val="19"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2238,6 +2326,9 @@
       <c:pivotFmt>
         <c:idx val="20"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2304,6 +2395,9 @@
       <c:pivotFmt>
         <c:idx val="21"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2370,6 +2464,9 @@
       <c:pivotFmt>
         <c:idx val="22"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2436,6 +2533,9 @@
       <c:pivotFmt>
         <c:idx val="23"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2502,6 +2602,9 @@
       <c:pivotFmt>
         <c:idx val="24"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2568,6 +2671,9 @@
       <c:pivotFmt>
         <c:idx val="25"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2634,6 +2740,9 @@
       <c:pivotFmt>
         <c:idx val="26"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2700,6 +2809,9 @@
       <c:pivotFmt>
         <c:idx val="27"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2766,6 +2878,9 @@
       <c:pivotFmt>
         <c:idx val="28"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2832,6 +2947,9 @@
       <c:pivotFmt>
         <c:idx val="29"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2898,6 +3016,9 @@
       <c:pivotFmt>
         <c:idx val="30"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2964,6 +3085,9 @@
       <c:pivotFmt>
         <c:idx val="31"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3030,6 +3154,9 @@
       <c:pivotFmt>
         <c:idx val="32"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3096,6 +3223,9 @@
       <c:pivotFmt>
         <c:idx val="33"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3162,6 +3292,9 @@
       <c:pivotFmt>
         <c:idx val="34"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3228,6 +3361,9 @@
       <c:pivotFmt>
         <c:idx val="35"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3294,6 +3430,9 @@
       <c:pivotFmt>
         <c:idx val="36"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3360,6 +3499,9 @@
       <c:pivotFmt>
         <c:idx val="37"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3426,6 +3568,9 @@
       <c:pivotFmt>
         <c:idx val="38"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3492,6 +3637,9 @@
       <c:pivotFmt>
         <c:idx val="39"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3558,6 +3706,9 @@
       <c:pivotFmt>
         <c:idx val="40"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3624,6 +3775,9 @@
       <c:pivotFmt>
         <c:idx val="41"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3690,6 +3844,9 @@
       <c:pivotFmt>
         <c:idx val="42"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3756,6 +3913,9 @@
       <c:pivotFmt>
         <c:idx val="43"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3822,6 +3982,9 @@
       <c:pivotFmt>
         <c:idx val="44"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3888,6 +4051,9 @@
       <c:pivotFmt>
         <c:idx val="45"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3954,6 +4120,9 @@
       <c:pivotFmt>
         <c:idx val="46"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4020,6 +4189,9 @@
       <c:pivotFmt>
         <c:idx val="47"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4086,6 +4258,9 @@
       <c:pivotFmt>
         <c:idx val="48"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4593,7 +4768,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Dashboard.xlsx]Comp entre cul vs dep vs soc!ComparaciónEntreServiciosCulturalesVsDeportivosVsSociales</c:name>
+    <c:name>[Dashboard(Recuperado automáticamente).xlsx]Comp entre cul vs dep vs soc!ComparaciónEntreServiciosCulturalesVsDeportivosVsSociales</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -5066,38 +5241,6 @@
           </a:ln>
           <a:effectLst/>
         </c:spPr>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-MX"/>
-            </a:p>
-          </c:txPr>
-        </c:dLbl>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -6230,7 +6373,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Dashboard.xlsx]Ranking de delegaciones!RankingDeDelegaciones</c:name>
+    <c:name>[Dashboard(Recuperado automáticamente).xlsx]Ranking de delegaciones!RankingDeDelegaciones</c:name>
     <c:fmtId val="2"/>
   </c:pivotSource>
   <c:chart>
@@ -6297,9 +6440,115 @@
         <c:idx val="1"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:lumMod val="80000"/>
-            </a:schemeClr>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -6342,6 +6591,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-6A5F-4888-AF57-DC71DDD60C90}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -6356,6 +6610,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-6A5F-4888-AF57-DC71DDD60C90}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -6370,6 +6629,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-6A5F-4888-AF57-DC71DDD60C90}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -6386,6 +6650,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-6A5F-4888-AF57-DC71DDD60C90}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -6402,6 +6671,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-6A5F-4888-AF57-DC71DDD60C90}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -6418,6 +6692,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-6A5F-4888-AF57-DC71DDD60C90}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -6435,6 +6714,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-6A5F-4888-AF57-DC71DDD60C90}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -6452,6 +6736,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-6A5F-4888-AF57-DC71DDD60C90}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -6469,6 +6758,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-6A5F-4888-AF57-DC71DDD60C90}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -9171,6 +9465,1378 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>754380</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectángulo: esquinas redondeadas 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1455E126-35E3-64B0-74EF-9539C250CDF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1546860" y="304800"/>
+          <a:ext cx="4091940" cy="1089660"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CuadroTexto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AA9D155-B202-BE03-C121-3275AB0BBA20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1607820" y="419100"/>
+          <a:ext cx="3954780" cy="312420"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1800" b="1">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Delegación con más servicios</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>784860</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectángulo: esquinas redondeadas 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{472A16AD-55BB-45DA-B3A6-1E291DE2AB5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1577340" y="1950720"/>
+          <a:ext cx="4091940" cy="1089660"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="CuadroTexto 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABC9A43E-8C39-4160-91BE-E1BC51F6A885}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1638300" y="2065020"/>
+          <a:ext cx="3954780" cy="312420"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1800" b="1">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Delegación con menos servicios</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>655320</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="'Ranking de delegaciones'!E34">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="CuadroTexto 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{681F35E1-A3F3-41BB-85EA-CE8349ED9BF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3825240" y="2430780"/>
+          <a:ext cx="1767840" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:fld id="{DD357D03-2B5F-443E-87A0-7A65FB514219}" type="TxLink">
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:pPr algn="ctr"/>
+            <a:t>55249</a:t>
+          </a:fld>
+          <a:endParaRPr lang="es-MX" sz="1400" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectángulo: esquinas redondeadas 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99702E67-9B5D-4EC1-ACBD-98618394CDBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6347460" y="266700"/>
+          <a:ext cx="4091940" cy="1089660"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="CuadroTexto 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FC6A63D-09D9-4DDC-8482-A90863D715CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6408420" y="381000"/>
+          <a:ext cx="3954780" cy="312420"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1800" b="1">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Servicio</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1800" b="1" baseline="0">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> más solicitado</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1800" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>739140</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectángulo: esquinas redondeadas 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EC0248D-EB84-4C8B-85BD-ABCA7218BE6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6286500" y="1897380"/>
+          <a:ext cx="4091940" cy="1089660"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="CuadroTexto 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36C36264-CCDF-4096-B3CD-236649DDDB55}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6347460" y="2011680"/>
+          <a:ext cx="3954780" cy="312420"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1800" b="1">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Total</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1800" b="1" baseline="0">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> de servicios</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1800" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>640080</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="'Ranking de Servicios'!E16">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="CuadroTexto 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{680396CA-F071-40FB-A229-3E21C5E9ED9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7254240" y="2369820"/>
+          <a:ext cx="2103120" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:fld id="{73561CD5-4F8D-4C7E-B681-88707DD3FB18}" type="TxLink">
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>56915689</a:t>
+          </a:fld>
+          <a:endParaRPr lang="es-MX" sz="1800" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="'Ranking de delegaciones'!D34">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="CuadroTexto 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{218B5F3B-AF3B-4B0A-899D-9E0BF4329C2E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1623060" y="2430780"/>
+          <a:ext cx="1889760" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:fld id="{17289592-5ED0-463A-8B4B-5C77C9640804}" type="TxLink">
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:pPr algn="ctr"/>
+            <a:t>Regional Oriente</a:t>
+          </a:fld>
+          <a:endParaRPr lang="es-MX" sz="1400" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>624840</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="'Ranking de delegaciones'!B28">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="CuadroTexto 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0618113B-8F2D-4DE1-B08E-EC156AA89D47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3794760" y="769620"/>
+          <a:ext cx="1767840" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:fld id="{50E00774-0124-44E7-BA7E-4D5884A39B98}" type="TxLink">
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:pPr algn="ctr"/>
+            <a:t>12806883</a:t>
+          </a:fld>
+          <a:endParaRPr lang="es-MX" sz="1400" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="'Ranking de delegaciones'!A28">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="CuadroTexto 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77278733-4FDC-4438-88ED-B9510EAF48FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1600200" y="769620"/>
+          <a:ext cx="1889760" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:fld id="{602BAB72-648C-40A5-8F51-EC6F8C7E9110}" type="TxLink">
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:pPr algn="ctr"/>
+            <a:t>Oficinas Centrales</a:t>
+          </a:fld>
+          <a:endParaRPr lang="es-MX" sz="1400" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>662940</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="'Ranking de Servicios'!E8">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="CuadroTexto 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D5DACA7-4763-422B-A40A-08AD48FAA136}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8587740" y="731520"/>
+          <a:ext cx="1767840" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:fld id="{FF2905A7-DF8B-43B9-9F6F-A1049135B0A5}" type="TxLink">
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>36375442</a:t>
+          </a:fld>
+          <a:endParaRPr lang="es-MX" sz="1400" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="'Ranking de Servicios'!D8">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="CuadroTexto 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1913509C-FE01-4796-8E19-5C453600F5ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6416040" y="731520"/>
+          <a:ext cx="1889760" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:fld id="{606645CA-79C5-4D31-B82D-489E6831CDAC}" type="TxLink">
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Serv. Culturales Derecho Hab Publ</a:t>
+          </a:fld>
+          <a:endParaRPr lang="es-MX" sz="1400" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="CuadroTexto 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D088F506-F6BE-ABE0-2CA3-FF5C384A37AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8214360" y="800100"/>
+          <a:ext cx="678180" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1400" b="1">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>con</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="CuadroTexto 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29C074E2-799A-4044-AA88-C4E3A7151771}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3383280" y="815340"/>
+          <a:ext cx="678180" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1400" b="1">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>con</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="CuadroTexto 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBC9B4B8-B026-4F57-904A-9A3BB13F899B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3390900" y="2491740"/>
+          <a:ext cx="678180" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1400" b="1">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>con</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Said Mariano" refreshedDate="45980.47015335648" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="494" xr:uid="{45697F6F-B6C1-4FB2-A6B4-D0194C73A538}">
   <cacheSource type="worksheet">
@@ -11430,6 +13096,36 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Said Mariano" refreshedDate="45982.533347337965" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="8" xr:uid="{71A40FA1-9934-4051-840D-BF1E7AA9F939}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Tabla3"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="Nombre Servicio" numFmtId="1">
+      <sharedItems count="8">
+        <s v="Serv. Culturales Derecho Hab Publ"/>
+        <s v="Serv. Deportivos Derecho Hab Publ"/>
+        <s v="Serv. Sociales Derecho Hab Publ"/>
+        <s v="Serv. Funerarios Derecho Hab Publ"/>
+        <s v="Serv. Sociales Pensionados Jubl"/>
+        <s v="Fome Deportivo Pensionados Jubl"/>
+        <s v="Serv. Culturales Pensionados Jubl"/>
+        <s v="Soci Comedores Pensionados Jubl"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Total de cada servicio" numFmtId="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="322484" maxValue="36375442"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="494">
   <r>
@@ -18351,8 +20047,45 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="8">
+  <r>
+    <x v="0"/>
+    <n v="36375442"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="11512451"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="661401"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="322484"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="2175717"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="1962313"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="3250887"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="654994"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1F62BD48-AAC3-4695-8D01-0E115DAB1328}" name="ServiciosDeportivosPorAño" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Años" colHeaderCaption="Nombre Oficina Representación">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1F62BD48-AAC3-4695-8D01-0E115DAB1328}" name="ServiciosDeportivosPorAño" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Años" colHeaderCaption="Nombre Oficina Representación">
   <location ref="A6:B21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" numFmtId="1" showAll="0">
@@ -19108,7 +20841,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{925D5B79-7889-4349-AA7F-C5C2592F1090}" name="ComparaciónEntreServiciosCulturalesVsDeportivosVsSociales" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11" rowHeaderCaption="Nombre Oficina Representación">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{925D5B79-7889-4349-AA7F-C5C2592F1090}" name="ComparaciónEntreServiciosCulturalesVsDeportivosVsSociales" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11" rowHeaderCaption="Nombre Oficina Representación">
   <location ref="A6:I7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField numFmtId="1" showAll="0"/>
@@ -19320,7 +21053,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{97A441A6-56C0-4FFA-911D-41686AFDD066}" name="RankingDeDelegaciones" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Nombre Oficina Representación">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{97A441A6-56C0-4FFA-911D-41686AFDD066}" name="RankingDeDelegaciones" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Nombre Oficina Representación">
   <location ref="A9:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField numFmtId="1" showAll="0"/>
@@ -21601,7 +23334,7 @@
   <dataFields count="1">
     <dataField name="Suma de todos los Servicios " fld="11" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
-  <chartFormats count="2">
+  <chartFormats count="11">
     <chartFormat chart="2" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -21619,6 +23352,114 @@
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="28"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="26"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="19"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="47"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="48"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="22"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="27"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -21645,6 +23486,336 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D6020FD5-92A0-48FE-8CAE-735B6AC6C5DD}" name="TablaDinámica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A33:B83" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="50">
+        <item x="0"/>
+        <item x="38"/>
+        <item x="1"/>
+        <item x="39"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="44"/>
+        <item x="36"/>
+        <item x="45"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="46"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="37"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="35"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="40"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="41"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="31"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="32"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField dataField="1" numFmtId="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="50">
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma de Suma de todos los Servicios" fld="11" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F2231237-FEAB-409D-B0B0-7D68E8795616}" name="TablaDinámica1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A7:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="9">
+        <item x="7"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma de Total de cada servicio" fld="1" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01004CAF-B0EE-4A4F-99F5-2C4E7F69B1DF}" name="Tabla1" displayName="Tabla1" ref="A1:L495" totalsRowShown="0">
   <autoFilter ref="A1:L495" xr:uid="{01004CAF-B0EE-4A4F-99F5-2C4E7F69B1DF}"/>
@@ -21652,20 +23823,31 @@
     <sortCondition descending="1" ref="L1:L495"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{E00903E2-5B95-4A2E-B89D-5B0052D7F544}" name="Año" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{E00903E2-5B95-4A2E-B89D-5B0052D7F544}" name="Año" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{6015B546-CCE8-49F7-AD82-A56721BEB06D}" name="Oficina Representación"/>
-    <tableColumn id="3" xr3:uid="{6C24FA5D-647C-4DF8-A6EA-66A6E6528CE5}" name="Serv. Culturales Derecho Hab Publ" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{5625FA80-061B-464D-B123-C974C04DA294}" name="Serv. Deportivos Derecho Hab Publ" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{24DE0E05-24AF-4FCC-9633-B84A75B97D9A}" name="Serv. Sociales Derecho Hab Publ" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{2AC1C74A-7627-48C3-AC0B-15FBB8351EE0}" name="Serv. Funerarios Derecho Hab Publ" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{3E1E2BD6-8333-4561-B9F1-248EFBB7920E}" name="Serv. Sociales Pensionados Jubl" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{2AC1B96B-1C99-43AF-AFED-47F1F4C408FD}" name="Fome Deportivo Pensionados Jubl" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{E70B6682-15CA-4E92-BD60-818587E36A59}" name="Serv. Culturales Pensionados Jubl" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{08067B72-2814-4712-B380-BB03A667992C}" name="Soci Comedores Pensionados Jubl" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{230A8DA6-C4FF-44BE-9A39-A60006ECF43E}" name="Fecha" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{859920B6-B83D-4724-917B-E5C66D0C0364}" name="Suma de todos los Servicios" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{6C24FA5D-647C-4DF8-A6EA-66A6E6528CE5}" name="Serv. Culturales Derecho Hab Publ" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{5625FA80-061B-464D-B123-C974C04DA294}" name="Serv. Deportivos Derecho Hab Publ" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{24DE0E05-24AF-4FCC-9633-B84A75B97D9A}" name="Serv. Sociales Derecho Hab Publ" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{2AC1C74A-7627-48C3-AC0B-15FBB8351EE0}" name="Serv. Funerarios Derecho Hab Publ" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{3E1E2BD6-8333-4561-B9F1-248EFBB7920E}" name="Serv. Sociales Pensionados Jubl" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{2AC1B96B-1C99-43AF-AFED-47F1F4C408FD}" name="Fome Deportivo Pensionados Jubl" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{E70B6682-15CA-4E92-BD60-818587E36A59}" name="Serv. Culturales Pensionados Jubl" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{08067B72-2814-4712-B380-BB03A667992C}" name="Soci Comedores Pensionados Jubl" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{230A8DA6-C4FF-44BE-9A39-A60006ECF43E}" name="Fecha" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{859920B6-B83D-4724-917B-E5C66D0C0364}" name="Suma de todos los Servicios" dataDxfId="2">
       <calculatedColumnFormula>SUM(Tabla1[[#This Row],[Serv. Culturales Derecho Hab Publ]:[Soci Comedores Pensionados Jubl]])</calculatedColumnFormula>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{943BA7B8-89FD-4590-985A-D669DB928326}" name="Tabla3" displayName="Tabla3" ref="B505:C513" totalsRowShown="0">
+  <autoFilter ref="B505:C513" xr:uid="{943BA7B8-89FD-4590-985A-D669DB928326}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{52308A83-3E58-4597-85E5-390E9550E560}" name="Nombre Servicio" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{DDDD0592-6492-4A2A-BC52-9B55A82E2E0F}" name="Total de cada servicio" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -21968,10 +24150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F449743-C6BA-4379-8C03-655115C7A180}">
-  <dimension ref="A1:L495"/>
+  <dimension ref="A1:L513"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView topLeftCell="A477" workbookViewId="0">
+      <selection activeCell="B508" sqref="B508"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41294,10 +43476,180 @@
         <v>0</v>
       </c>
     </row>
+    <row r="496" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F496" s="2"/>
+      <c r="J496" s="2"/>
+      <c r="L496" s="2"/>
+    </row>
+    <row r="497" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F497" s="2"/>
+      <c r="J497" s="2"/>
+      <c r="L497" s="2"/>
+    </row>
+    <row r="498" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C498" s="2" t="str">
+        <f>Tabla1[[#Headers],[Serv. Culturales Derecho Hab Publ]]</f>
+        <v>Serv. Culturales Derecho Hab Publ</v>
+      </c>
+      <c r="D498" s="2" t="str">
+        <f>Tabla1[[#Headers],[Serv. Deportivos Derecho Hab Publ]]</f>
+        <v>Serv. Deportivos Derecho Hab Publ</v>
+      </c>
+      <c r="E498" s="2" t="str">
+        <f>Tabla1[[#Headers],[Serv. Sociales Derecho Hab Publ]]</f>
+        <v>Serv. Sociales Derecho Hab Publ</v>
+      </c>
+      <c r="F498" s="2" t="str">
+        <f>Tabla1[[#Headers],[Serv. Funerarios Derecho Hab Publ]]</f>
+        <v>Serv. Funerarios Derecho Hab Publ</v>
+      </c>
+      <c r="G498" s="2" t="str">
+        <f>Tabla1[[#Headers],[Serv. Sociales Pensionados Jubl]]</f>
+        <v>Serv. Sociales Pensionados Jubl</v>
+      </c>
+      <c r="H498" s="2" t="str">
+        <f>Tabla1[[#Headers],[Fome Deportivo Pensionados Jubl]]</f>
+        <v>Fome Deportivo Pensionados Jubl</v>
+      </c>
+      <c r="I498" s="2" t="str">
+        <f>Tabla1[[#Headers],[Serv. Culturales Pensionados Jubl]]</f>
+        <v>Serv. Culturales Pensionados Jubl</v>
+      </c>
+      <c r="J498" s="2" t="str">
+        <f>Tabla1[[#Headers],[Soci Comedores Pensionados Jubl]]</f>
+        <v>Soci Comedores Pensionados Jubl</v>
+      </c>
+    </row>
+    <row r="499" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B499" t="s">
+        <v>81</v>
+      </c>
+      <c r="C499" s="2">
+        <f>SUM(Tabla1[Serv. Culturales Derecho Hab Publ])</f>
+        <v>36375442</v>
+      </c>
+      <c r="D499" s="2">
+        <f>SUM(Tabla1[Serv. Deportivos Derecho Hab Publ])</f>
+        <v>11512451</v>
+      </c>
+      <c r="E499" s="2">
+        <f>SUM(Tabla1[Serv. Sociales Derecho Hab Publ])</f>
+        <v>661401</v>
+      </c>
+      <c r="F499" s="2">
+        <f>SUM(Tabla1[Serv. Funerarios Derecho Hab Publ])</f>
+        <v>322484</v>
+      </c>
+      <c r="G499" s="2">
+        <f>SUM(Tabla1[Serv. Sociales Pensionados Jubl])</f>
+        <v>2175717</v>
+      </c>
+      <c r="H499" s="2">
+        <f>SUM(Tabla1[Fome Deportivo Pensionados Jubl])</f>
+        <v>1962313</v>
+      </c>
+      <c r="I499" s="2">
+        <f>SUM(Tabla1[Serv. Culturales Pensionados Jubl])</f>
+        <v>3250887</v>
+      </c>
+      <c r="J499" s="2">
+        <f>SUM(Tabla1[Soci Comedores Pensionados Jubl])</f>
+        <v>654994</v>
+      </c>
+    </row>
+    <row r="505" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B505" t="s">
+        <v>82</v>
+      </c>
+      <c r="C505" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="506" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B506" s="2" t="str">
+        <f>Tabla1[[#Headers],[Serv. Culturales Derecho Hab Publ]]</f>
+        <v>Serv. Culturales Derecho Hab Publ</v>
+      </c>
+      <c r="C506" s="2">
+        <f>SUM(Tabla1[Serv. Culturales Derecho Hab Publ])</f>
+        <v>36375442</v>
+      </c>
+    </row>
+    <row r="507" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B507" s="2" t="str">
+        <f>Tabla1[[#Headers],[Serv. Deportivos Derecho Hab Publ]]</f>
+        <v>Serv. Deportivos Derecho Hab Publ</v>
+      </c>
+      <c r="C507" s="2">
+        <f>SUM(Tabla1[Serv. Deportivos Derecho Hab Publ])</f>
+        <v>11512451</v>
+      </c>
+    </row>
+    <row r="508" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B508" s="2" t="str">
+        <f>Tabla1[[#Headers],[Serv. Sociales Derecho Hab Publ]]</f>
+        <v>Serv. Sociales Derecho Hab Publ</v>
+      </c>
+      <c r="C508" s="2">
+        <f>SUM(Tabla1[Serv. Sociales Derecho Hab Publ])</f>
+        <v>661401</v>
+      </c>
+    </row>
+    <row r="509" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B509" s="2" t="str">
+        <f>Tabla1[[#Headers],[Serv. Funerarios Derecho Hab Publ]]</f>
+        <v>Serv. Funerarios Derecho Hab Publ</v>
+      </c>
+      <c r="C509" s="2">
+        <f>SUM(Tabla1[Serv. Funerarios Derecho Hab Publ])</f>
+        <v>322484</v>
+      </c>
+    </row>
+    <row r="510" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B510" s="2" t="str">
+        <f>Tabla1[[#Headers],[Serv. Sociales Pensionados Jubl]]</f>
+        <v>Serv. Sociales Pensionados Jubl</v>
+      </c>
+      <c r="C510" s="2">
+        <f>SUM(Tabla1[Serv. Sociales Pensionados Jubl])</f>
+        <v>2175717</v>
+      </c>
+    </row>
+    <row r="511" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B511" s="2" t="str">
+        <f>Tabla1[[#Headers],[Fome Deportivo Pensionados Jubl]]</f>
+        <v>Fome Deportivo Pensionados Jubl</v>
+      </c>
+      <c r="C511" s="2">
+        <f>SUM(Tabla1[Fome Deportivo Pensionados Jubl])</f>
+        <v>1962313</v>
+      </c>
+    </row>
+    <row r="512" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B512" s="2" t="str">
+        <f>Tabla1[[#Headers],[Serv. Culturales Pensionados Jubl]]</f>
+        <v>Serv. Culturales Pensionados Jubl</v>
+      </c>
+      <c r="C512" s="2">
+        <f>SUM(Tabla1[Serv. Culturales Pensionados Jubl])</f>
+        <v>3250887</v>
+      </c>
+    </row>
+    <row r="513" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B513" s="2" t="str">
+        <f>Tabla1[[#Headers],[Soci Comedores Pensionados Jubl]]</f>
+        <v>Soci Comedores Pensionados Jubl</v>
+      </c>
+      <c r="C513" s="2">
+        <f>SUM(Tabla1[Soci Comedores Pensionados Jubl])</f>
+        <v>654994</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -41306,7 +43658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56573DCE-1102-4670-B2C5-59B84C64109B}">
   <dimension ref="A2:F25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -41624,16 +43976,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803E057B-2FFD-452E-9801-D0EF6EE0D059}">
-  <dimension ref="A2:J20"/>
+  <dimension ref="A2:J83"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.88671875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
@@ -42197,12 +44549,564 @@
         <v>29655916</v>
       </c>
     </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
+        <f>A19</f>
+        <v>Oficinas Centrales</v>
+      </c>
+      <c r="B28">
+        <f>GETPIVOTDATA("Suma de todos los Servicios",$A$9,"Oficina Representación","Oficinas Centrales")</f>
+        <v>12806883</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="2">
+        <v>55249</v>
+      </c>
+      <c r="D34" t="str">
+        <f>A34</f>
+        <v>Regional Oriente</v>
+      </c>
+      <c r="E34">
+        <f>GETPIVOTDATA("Suma de todos los Servicios",$A$33,"Oficina Representación","Regional Oriente")</f>
+        <v>55249</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="2">
+        <v>110312</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="2">
+        <v>139866</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="2">
+        <v>172802</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="2">
+        <v>236848</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="2">
+        <v>330258</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="2">
+        <v>367601</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="2">
+        <v>379617</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="2">
+        <v>388326</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="2">
+        <v>454525</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="2">
+        <v>464037</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="2">
+        <v>514526</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="2">
+        <v>541003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="2">
+        <v>604570</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="2">
+        <v>624538</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="2">
+        <v>630996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="2">
+        <v>705652</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="2">
+        <v>721599</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="2">
+        <v>749396</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="2">
+        <v>792076</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" s="2">
+        <v>806518</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="2">
+        <v>833184</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" s="2">
+        <v>858610</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="2">
+        <v>888123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" s="2">
+        <v>904262</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" s="2">
+        <v>908129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B60" s="2">
+        <v>918381</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" s="2">
+        <v>937351</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" s="2">
+        <v>944130</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="2">
+        <v>960342</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64" s="2">
+        <v>991542</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B65" s="2">
+        <v>993249</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66" s="2">
+        <v>993584</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67" s="2">
+        <v>996808</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B68" s="2">
+        <v>1004872</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B69" s="2">
+        <v>1009606</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" s="2">
+        <v>1061964</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B71" s="2">
+        <v>1118233</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" s="2">
+        <v>1147088</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B73" s="2">
+        <v>1151362</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" s="2">
+        <v>1329318</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B75" s="2">
+        <v>1396246</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B76" s="2">
+        <v>1544155</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B77" s="2">
+        <v>1700361</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B78" s="2">
+        <v>1853200</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B79" s="2">
+        <v>2141268</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B80" s="2">
+        <v>2824608</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B81" s="2">
+        <v>2908515</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B82" s="2">
+        <v>12806883</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B83" s="2">
+        <v>56915689</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F6:J7"/>
     <mergeCell ref="B2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEFD455-FE5D-4DB9-B672-24C684C812DC}">
+  <dimension ref="A7:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="2">
+        <v>36375442</v>
+      </c>
+      <c r="D8" t="str">
+        <f>A8</f>
+        <v>Serv. Culturales Derecho Hab Publ</v>
+      </c>
+      <c r="E8">
+        <f>GETPIVOTDATA("Total de cada servicio",$A$7,"Nombre Servicio","Serv. Culturales Derecho Hab Publ")</f>
+        <v>36375442</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="2">
+        <v>11512451</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3250887</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2175717</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1962313</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="2">
+        <v>661401</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2">
+        <v>654994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="2">
+        <v>322484</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="2">
+        <v>56915689</v>
+      </c>
+      <c r="E16">
+        <f>GETPIVOTDATA("Total de cada servicio",$A$7)</f>
+        <v>56915689</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E4A35B-1DEE-4E63-B176-45BEFEC88566}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Creación de gráfico de pastel
</commit_message>
<xml_diff>
--- a/Dashboard/Dashboard.xlsx
+++ b/Dashboard/Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\servicios_cul_soci_depor_recre\Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15019FF8-4902-4F16-BE4D-33FA2BC777E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C5303E-6425-40A1-B50A-679E2410A70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" activeTab="5" xr2:uid="{0F6DE12B-782F-43E4-BCEE-D62EF1718F31}"/>
   </bookViews>
@@ -22,10 +22,9 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId7"/>
-    <pivotCache cacheId="5" r:id="rId8"/>
+    <pivotCache cacheId="2" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -907,7 +906,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Dashboard(Recuperado automáticamente).xlsx]Servios deportivos por año!ServiciosDeportivosPorAño</c:name>
+    <c:name>[Dashboard.xlsx]Servios deportivos por año!ServiciosDeportivosPorAño</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -4768,7 +4767,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Dashboard(Recuperado automáticamente).xlsx]Comp entre cul vs dep vs soc!ComparaciónEntreServiciosCulturalesVsDeportivosVsSociales</c:name>
+    <c:name>[Dashboard.xlsx]Comp entre cul vs dep vs soc!ComparaciónEntreServiciosCulturalesVsDeportivosVsSociales</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -6373,7 +6372,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Dashboard(Recuperado automáticamente).xlsx]Ranking de delegaciones!RankingDeDelegaciones</c:name>
+    <c:name>[Dashboard.xlsx]Ranking de delegaciones!RankingDeDelegaciones</c:name>
     <c:fmtId val="2"/>
   </c:pivotSource>
   <c:chart>
@@ -7070,6 +7069,436 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Dashboard.xlsx]Ranking de Servicios!TablaDinámica1</c:name>
+    <c:fmtId val="6"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:separator>
+</c:separator>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ranking de Servicios'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:explosion val="3"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:separator>
+</c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst>
+                  <a:glow rad="127000">
+                    <a:schemeClr val="bg2">
+                      <a:lumMod val="90000"/>
+                    </a:schemeClr>
+                  </a:glow>
+                </a:effectLst>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ranking de Servicios'!$A$8:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Serv. Culturales Derecho Hab Publ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Serv. Deportivos Derecho Hab Publ</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Serv. Culturales Pensionados Jubl</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Serv. Sociales Pensionados Jubl</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fome Deportivo Pensionados Jubl</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Serv. Sociales Derecho Hab Publ</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Soci Comedores Pensionados Jubl</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Serv. Funerarios Derecho Hab Publ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ranking de Servicios'!$B$8:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>36375442</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11512451</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3250887</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2175717</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1962313</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>661401</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>654994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>322484</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-685C-4B01-8954-9AA576FB6BF8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -7155,6 +7584,46 @@
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent5"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -8700,6 +9169,525 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -9469,6 +10457,47 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2415540</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79D90A1A-D24F-D04B-3C4B-2BAD344D5832}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>754380</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -10183,6 +11212,7 @@
               <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
+            <a:pPr algn="ctr"/>
             <a:t>56915689</a:t>
           </a:fld>
           <a:endParaRPr lang="es-MX" sz="1800" b="1">
@@ -10517,6 +11547,7 @@
               <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
+            <a:pPr algn="ctr"/>
             <a:t>36375442</a:t>
           </a:fld>
           <a:endParaRPr lang="es-MX" sz="1400" b="1">
@@ -10600,6 +11631,7 @@
               <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
+            <a:pPr algn="ctr"/>
             <a:t>Serv. Culturales Derecho Hab Publ</a:t>
           </a:fld>
           <a:endParaRPr lang="es-MX" sz="1400" b="1">
@@ -20085,7 +21117,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1F62BD48-AAC3-4695-8D01-0E115DAB1328}" name="ServiciosDeportivosPorAño" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Años" colHeaderCaption="Nombre Oficina Representación">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1F62BD48-AAC3-4695-8D01-0E115DAB1328}" name="ServiciosDeportivosPorAño" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Años" colHeaderCaption="Nombre Oficina Representación">
   <location ref="A6:B21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" numFmtId="1" showAll="0">
@@ -20841,7 +21873,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{925D5B79-7889-4349-AA7F-C5C2592F1090}" name="ComparaciónEntreServiciosCulturalesVsDeportivosVsSociales" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11" rowHeaderCaption="Nombre Oficina Representación">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{925D5B79-7889-4349-AA7F-C5C2592F1090}" name="ComparaciónEntreServiciosCulturalesVsDeportivosVsSociales" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11" rowHeaderCaption="Nombre Oficina Representación">
   <location ref="A6:I7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField numFmtId="1" showAll="0"/>
@@ -21053,7 +22085,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{97A441A6-56C0-4FFA-911D-41686AFDD066}" name="RankingDeDelegaciones" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Nombre Oficina Representación">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{97A441A6-56C0-4FFA-911D-41686AFDD066}" name="RankingDeDelegaciones" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Nombre Oficina Representación">
   <location ref="A9:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField numFmtId="1" showAll="0"/>
@@ -23487,7 +24519,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D6020FD5-92A0-48FE-8CAE-735B6AC6C5DD}" name="TablaDinámica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D6020FD5-92A0-48FE-8CAE-735B6AC6C5DD}" name="TablaDinámica1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A33:B83" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField numFmtId="1" showAll="0"/>
@@ -23739,7 +24771,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F2231237-FEAB-409D-B0B0-7D68E8795616}" name="TablaDinámica1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F2231237-FEAB-409D-B0B0-7D68E8795616}" name="TablaDinámica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
   <location ref="A7:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -23804,6 +24836,26 @@
   <dataFields count="1">
     <dataField name="Suma de Total de cada servicio" fld="1" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -24153,7 +25205,7 @@
   <dimension ref="A1:L513"/>
   <sheetViews>
     <sheetView topLeftCell="A477" workbookViewId="0">
-      <selection activeCell="B508" sqref="B508"/>
+      <selection activeCell="E504" sqref="E504"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43875,7 +44927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB971FC3-37E4-4473-BE72-831CFD6103DC}">
   <dimension ref="A2:I60"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
@@ -44989,14 +46041,363 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEFD455-FE5D-4DB9-B672-24C684C812DC}">
   <dimension ref="A7:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="36" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="36" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="36" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="36" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="36" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="56" max="57" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="36" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="64" max="65" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="36" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="72" max="73" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="36" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="80" max="81" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="36" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="88" max="89" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="36" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="96" max="97" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="36" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="104" max="105" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="36" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="112" max="113" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="36" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="120" max="121" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="36" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="128" max="129" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="36" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="136" max="137" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="36" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="144" max="145" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="36" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="152" max="153" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="155" max="155" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="156" max="156" width="36" bestFit="1" customWidth="1"/>
+    <col min="157" max="157" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="159" max="159" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="160" max="161" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="163" max="163" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="164" max="164" width="36" bestFit="1" customWidth="1"/>
+    <col min="165" max="165" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="168" max="169" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="170" max="170" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="171" max="171" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="172" max="172" width="36" bestFit="1" customWidth="1"/>
+    <col min="173" max="173" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="174" max="174" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="175" max="175" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="176" max="177" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="178" max="178" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="179" max="179" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="180" max="180" width="36" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="184" max="185" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="187" max="187" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="36" bestFit="1" customWidth="1"/>
+    <col min="189" max="189" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="190" max="190" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="191" max="191" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="192" max="193" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="194" max="194" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="195" max="195" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="196" max="196" width="36" bestFit="1" customWidth="1"/>
+    <col min="197" max="197" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="198" max="198" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="199" max="199" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="200" max="201" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="202" max="202" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="204" max="204" width="36" bestFit="1" customWidth="1"/>
+    <col min="205" max="205" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="206" max="206" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="207" max="207" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="208" max="209" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="210" max="210" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="211" max="211" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="212" max="212" width="36" bestFit="1" customWidth="1"/>
+    <col min="213" max="213" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="214" max="214" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="215" max="215" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="216" max="217" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="218" max="218" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="219" max="219" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="220" max="220" width="36" bestFit="1" customWidth="1"/>
+    <col min="221" max="221" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="224" max="225" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="226" max="226" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="227" max="227" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="228" max="228" width="36" bestFit="1" customWidth="1"/>
+    <col min="229" max="229" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="230" max="230" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="231" max="231" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="232" max="233" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="234" max="234" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="235" max="235" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="236" max="236" width="36" bestFit="1" customWidth="1"/>
+    <col min="237" max="237" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="238" max="238" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="239" max="239" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="240" max="241" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="242" max="242" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="243" max="243" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="244" max="244" width="36" bestFit="1" customWidth="1"/>
+    <col min="245" max="245" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="246" max="246" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="247" max="247" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="248" max="249" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="250" max="250" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="251" max="251" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="252" max="252" width="36" bestFit="1" customWidth="1"/>
+    <col min="253" max="253" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="254" max="254" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="255" max="255" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="256" max="257" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="36" bestFit="1" customWidth="1"/>
+    <col min="261" max="261" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="262" max="262" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="263" max="263" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="264" max="265" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="266" max="266" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="267" max="267" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="268" max="268" width="36" bestFit="1" customWidth="1"/>
+    <col min="269" max="269" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="270" max="270" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="271" max="271" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="272" max="273" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="274" max="274" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="275" max="275" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="276" max="276" width="36" bestFit="1" customWidth="1"/>
+    <col min="277" max="277" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="278" max="278" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="279" max="279" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="280" max="281" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="282" max="282" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="283" max="283" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="284" max="284" width="36" bestFit="1" customWidth="1"/>
+    <col min="285" max="285" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="286" max="286" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="287" max="287" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="288" max="289" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="290" max="290" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="291" max="291" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="292" max="292" width="36" bestFit="1" customWidth="1"/>
+    <col min="293" max="293" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="294" max="294" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="295" max="295" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="296" max="297" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="298" max="298" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="299" max="299" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="300" max="300" width="36" bestFit="1" customWidth="1"/>
+    <col min="301" max="301" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="302" max="302" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="303" max="303" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="304" max="305" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="306" max="306" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="307" max="307" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="308" max="308" width="36" bestFit="1" customWidth="1"/>
+    <col min="309" max="309" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="310" max="310" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="311" max="311" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="312" max="313" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="314" max="314" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="315" max="315" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="316" max="316" width="36" bestFit="1" customWidth="1"/>
+    <col min="317" max="317" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="318" max="318" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="319" max="319" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="320" max="321" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="322" max="322" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="323" max="323" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="324" max="324" width="36" bestFit="1" customWidth="1"/>
+    <col min="325" max="325" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="326" max="326" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="327" max="327" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="328" max="329" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="330" max="330" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="331" max="331" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="332" max="332" width="36" bestFit="1" customWidth="1"/>
+    <col min="333" max="333" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="334" max="334" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="335" max="335" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="336" max="337" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="338" max="338" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="339" max="339" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="340" max="340" width="36" bestFit="1" customWidth="1"/>
+    <col min="341" max="341" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="342" max="342" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="343" max="343" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="344" max="345" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="346" max="346" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="347" max="347" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="348" max="348" width="36" bestFit="1" customWidth="1"/>
+    <col min="349" max="349" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="350" max="350" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="351" max="351" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="352" max="353" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="354" max="354" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="355" max="355" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="356" max="356" width="36" bestFit="1" customWidth="1"/>
+    <col min="357" max="357" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="358" max="358" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="359" max="359" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="360" max="361" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="362" max="362" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="363" max="363" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="364" max="364" width="36" bestFit="1" customWidth="1"/>
+    <col min="365" max="365" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="366" max="366" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="367" max="367" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="368" max="369" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="370" max="370" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="371" max="371" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="372" max="372" width="36" bestFit="1" customWidth="1"/>
+    <col min="373" max="373" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="374" max="374" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="375" max="375" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="376" max="377" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="378" max="378" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="379" max="379" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="380" max="380" width="36" bestFit="1" customWidth="1"/>
+    <col min="381" max="381" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="382" max="382" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="383" max="383" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="384" max="385" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="386" max="386" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="387" max="387" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="388" max="388" width="36" bestFit="1" customWidth="1"/>
+    <col min="389" max="389" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="390" max="390" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="391" max="391" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="392" max="393" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="394" max="394" width="42.5546875" bestFit="1" customWidth="1"/>
+    <col min="395" max="395" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="396" max="396" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="397" max="397" width="43" bestFit="1" customWidth="1"/>
+    <col min="398" max="398" width="40.21875" bestFit="1" customWidth="1"/>
+    <col min="399" max="399" width="42" bestFit="1" customWidth="1"/>
+    <col min="400" max="401" width="42.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -45093,6 +46494,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -45101,7 +46503,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feat: Creación de plantilla para el Dashboard
</commit_message>
<xml_diff>
--- a/Dashboard/Dashboard.xlsx
+++ b/Dashboard/Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\servicios_cul_soci_depor_recre\Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C5303E-6425-40A1-B50A-679E2410A70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181634E4-9B94-47B4-93D1-4CAF0B1EF0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" activeTab="5" xr2:uid="{0F6DE12B-782F-43E4-BCEE-D62EF1718F31}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{0F6DE12B-782F-43E4-BCEE-D62EF1718F31}"/>
   </bookViews>
   <sheets>
     <sheet name="servicios_cult_soc_dep_rec_isss" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="Ranking de delegaciones" sheetId="4" r:id="rId4"/>
     <sheet name="Ranking de Servicios" sheetId="6" r:id="rId5"/>
     <sheet name="KPI's" sheetId="5" r:id="rId6"/>
+    <sheet name="Dasboard" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId7"/>
-    <pivotCache cacheId="1" r:id="rId8"/>
+    <pivotCache cacheId="2" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId9"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -11869,6 +11870,371 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>16934</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectángulo 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CB95077-019B-776F-4808-5F5AE9CB3788}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9525" y="19050"/>
+          <a:ext cx="20935950" cy="902759"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>169335</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>733424</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>177801</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectángulo: esquinas redondeadas 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D919ED6F-68FC-214C-1580-AD7158119916}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2962275" y="1074210"/>
+          <a:ext cx="14373224" cy="2542116"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>33867</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>8466</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectángulo: esquinas redondeadas 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7CD1729-C996-D9F3-B9D8-D8EFE98BE8BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1151467"/>
+          <a:ext cx="2396066" cy="5765800"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>629708</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>160868</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>275168</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>113242</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectángulo: esquinas redondeadas 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4D368C1-7846-44F6-A10E-4FAAAC7608BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3001433" y="3780368"/>
+          <a:ext cx="4388910" cy="2847974"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>737659</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>32809</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectángulo: esquinas redondeadas 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F1A988F-BACB-44D8-BA75-3E0FB626005D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7852834" y="3833284"/>
+          <a:ext cx="4367741" cy="2789766"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>250826</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>140758</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>688977</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>83608</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectángulo: esquinas redondeadas 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46E727AA-3279-4BFD-8C51-67F7F3A3D412}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12900026" y="3760258"/>
+          <a:ext cx="4391026" cy="2838450"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Said Mariano" refreshedDate="45980.47015335648" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="494" xr:uid="{45697F6F-B6C1-4FB2-A6B4-D0194C73A538}">
   <cacheSource type="worksheet">
@@ -24836,16 +25202,7 @@
   <dataFields count="1">
     <dataField name="Suma de Total de cada servicio" fld="1" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
+  <chartFormats count="1">
     <chartFormat chart="6" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -46502,8 +46859,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E4A35B-1DEE-4E63-B176-45BEFEC88566}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2626B9-BEDB-407F-B6C7-68E4D543C3D7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feaT: Se agregaron los KPI's y el título del Dashboard
</commit_message>
<xml_diff>
--- a/Dashboard/Dashboard.xlsx
+++ b/Dashboard/Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\servicios_cul_soci_depor_recre\Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8623C3A-4845-4978-95C3-2465BCF851BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC8CED6-4763-4400-A6F6-74B133071EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" firstSheet="2" activeTab="6" xr2:uid="{0F6DE12B-782F-43E4-BCEE-D62EF1718F31}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
     <pivotCache cacheId="1" r:id="rId9"/>
   </pivotCaches>
 </workbook>
@@ -7150,6 +7150,118 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -7184,6 +7296,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-F240-47C8-ACDE-536DB06B4568}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -7199,6 +7316,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-F240-47C8-ACDE-536DB06B4568}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -7214,6 +7336,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-F240-47C8-ACDE-536DB06B4568}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -7229,6 +7356,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-F240-47C8-ACDE-536DB06B4568}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -7244,6 +7376,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-F240-47C8-ACDE-536DB06B4568}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -7259,6 +7396,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-F240-47C8-ACDE-536DB06B4568}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -7276,6 +7418,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-F240-47C8-ACDE-536DB06B4568}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -7293,6 +7440,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-F240-47C8-ACDE-536DB06B4568}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -23247,6 +23399,1206 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>777240</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CuadroTexto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5070F730-A388-FA3A-C892-B9D0C4DECA29}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="121920" y="220980"/>
+          <a:ext cx="17297400" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="2400" b="1">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>ISSSTE: Evaluación de Servicios Culturales, Deportivos y Sociales a Nivel Nacional (2013 - 2025)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="CuadroTexto 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB17011D-98B6-49DD-8403-A54240E3B2D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4107180" y="1028700"/>
+          <a:ext cx="2247900" cy="312420"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1800" b="1">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Total</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1800" b="1" baseline="0">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> de servicios</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1800" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="'Ranking de Servicios'!E16">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="CuadroTexto 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B60A494A-2C76-4E7F-913F-44F36029D2C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4610100" y="1234440"/>
+          <a:ext cx="1310640" cy="327660"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:fld id="{73561CD5-4F8D-4C7E-B681-88707DD3FB18}" type="TxLink">
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:pPr algn="ctr"/>
+            <a:t>56915689</a:t>
+          </a:fld>
+          <a:endParaRPr lang="es-MX" sz="1800" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>640080</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="CuadroTexto 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63F4D61A-C99E-46F7-93DB-6D7FA2BF4BC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6979920" y="1013460"/>
+          <a:ext cx="3048000" cy="312420"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1400" b="1">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Delegación con más servicios</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>34312</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>784860</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="'Ranking de delegaciones'!B28">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="CuadroTexto 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20CE04F0-7C81-42F8-8CC6-C14EF35FA01A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8751592" y="1219200"/>
+          <a:ext cx="1543028" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:fld id="{50E00774-0124-44E7-BA7E-4D5884A39B98}" type="TxLink">
+            <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:pPr algn="ctr"/>
+            <a:t>12806883</a:t>
+          </a:fld>
+          <a:endParaRPr lang="es-MX" sz="1000" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590836</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>655320</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="'Ranking de delegaciones'!A28">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="CuadroTexto 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35F3BE94-4320-4318-8306-014D35B353FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6930676" y="1211580"/>
+          <a:ext cx="1649444" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:fld id="{602BAB72-648C-40A5-8F51-EC6F8C7E9110}" type="TxLink">
+            <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:pPr algn="ctr"/>
+            <a:t>Oficinas Centrales</a:t>
+          </a:fld>
+          <a:endParaRPr lang="es-MX" sz="1000" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>375802</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>175259</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="CuadroTexto 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDD6571C-2D19-496C-81DB-73A7AA499C47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8300602" y="1295400"/>
+          <a:ext cx="591937" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1000" b="1">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>con</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>662940</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="CuadroTexto 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB1BFC0D-52CB-4D8D-9C10-4E75CDD7F142}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10317480" y="975360"/>
+          <a:ext cx="3025140" cy="312420"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1400" b="1">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Delegación con menos servicios</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="'Ranking de delegaciones'!E34">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="CuadroTexto 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01826767-4494-4D18-AA61-48681B6CB96F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12115800" y="1211580"/>
+          <a:ext cx="1767840" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:fld id="{DD357D03-2B5F-443E-87A0-7A65FB514219}" type="TxLink">
+            <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:pPr algn="ctr"/>
+            <a:t>55249</a:t>
+          </a:fld>
+          <a:endParaRPr lang="es-MX" sz="1000" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>708660</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="'Ranking de delegaciones'!D34">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="CuadroTexto 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84265A11-659A-42ED-ACF0-D1042A9CA41D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9913620" y="1211580"/>
+          <a:ext cx="1889760" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:fld id="{17289592-5ED0-463A-8B4B-5C77C9640804}" type="TxLink">
+            <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:pPr algn="ctr"/>
+            <a:t>Regional Oriente</a:t>
+          </a:fld>
+          <a:endParaRPr lang="es-MX" sz="1000" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="CuadroTexto 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EA25C03-34B7-4845-A16D-EB6F83A13937}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11681460" y="1272540"/>
+          <a:ext cx="678180" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1000" b="1">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>con</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="CuadroTexto 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1C77B70-CE1B-4994-8EC1-A627F8DE3B9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12938760" y="1043940"/>
+          <a:ext cx="3954780" cy="312420"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1400" b="1">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Servicio</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1400" b="1" baseline="0">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> más solicitado</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1400" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="'Ranking de Servicios'!E8">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="CuadroTexto 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{813A0E44-07CA-41A6-8397-EEC5038415B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15262860" y="1211580"/>
+          <a:ext cx="1767840" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:fld id="{FF2905A7-DF8B-43B9-9F6F-A1049135B0A5}" type="TxLink">
+            <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:pPr algn="ctr"/>
+            <a:t>36375442</a:t>
+          </a:fld>
+          <a:endParaRPr lang="es-MX" sz="1000" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>716280</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="'Ranking de Servicios'!D8">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="CuadroTexto 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A13B6752-668A-46BC-8E89-C92FD129732B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13091160" y="1211580"/>
+          <a:ext cx="1889760" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:fld id="{606645CA-79C5-4D31-B82D-489E6831CDAC}" type="TxLink">
+            <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:pPr algn="ctr"/>
+            <a:t>Serv. Culturales Derecho Hab Publ</a:t>
+          </a:fld>
+          <a:endParaRPr lang="es-MX" sz="1000" b="1">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Tahoma" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>624840</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="CuadroTexto 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4338EF03-C5F9-4F0A-A888-F84177C1024A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14889480" y="1280160"/>
+          <a:ext cx="678180" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1000" b="1">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>con</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -32498,7 +33850,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1F62BD48-AAC3-4695-8D01-0E115DAB1328}" name="ServiciosDeportivosPorAño" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Años" colHeaderCaption="Nombre Oficina Representación">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1F62BD48-AAC3-4695-8D01-0E115DAB1328}" name="ServiciosDeportivosPorAño" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Años" colHeaderCaption="Nombre Oficina Representación">
   <location ref="A6:B21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" numFmtId="1" showAll="0">
@@ -33263,7 +34615,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{925D5B79-7889-4349-AA7F-C5C2592F1090}" name="ComparaciónEntreServiciosCulturalesVsDeportivosVsSociales" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14" rowHeaderCaption="Nombre Oficina Representación">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{925D5B79-7889-4349-AA7F-C5C2592F1090}" name="ComparaciónEntreServiciosCulturalesVsDeportivosVsSociales" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14" rowHeaderCaption="Nombre Oficina Representación">
   <location ref="A6:I7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField numFmtId="1" showAll="0"/>
@@ -33547,7 +34899,259 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{97A441A6-56C0-4FFA-911D-41686AFDD066}" name="RankingDeDelegaciones" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11" rowHeaderCaption="Nombre Oficina Representación">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D6020FD5-92A0-48FE-8CAE-735B6AC6C5DD}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A33:B83" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="50">
+        <item x="0"/>
+        <item x="38"/>
+        <item x="1"/>
+        <item x="39"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="44"/>
+        <item x="36"/>
+        <item x="45"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="46"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="37"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="35"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="40"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="41"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="31"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="32"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField dataField="1" numFmtId="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="50">
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma de Suma de todos los Servicios" fld="11" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{97A441A6-56C0-4FFA-911D-41686AFDD066}" name="RankingDeDelegaciones" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11" rowHeaderCaption="Nombre Oficina Representación">
   <location ref="A9:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField numFmtId="1" showAll="0"/>
@@ -36109,258 +37713,6 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D6020FD5-92A0-48FE-8CAE-735B6AC6C5DD}" name="TablaDinámica1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A33:B83" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField numFmtId="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="50">
-        <item x="0"/>
-        <item x="38"/>
-        <item x="1"/>
-        <item x="39"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="44"/>
-        <item x="36"/>
-        <item x="45"/>
-        <item x="47"/>
-        <item x="48"/>
-        <item x="46"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="37"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="35"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="40"/>
-        <item x="42"/>
-        <item x="43"/>
-        <item x="41"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="31"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="32"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField numFmtId="1" showAll="0"/>
-    <pivotField numFmtId="1" showAll="0"/>
-    <pivotField numFmtId="1" showAll="0"/>
-    <pivotField numFmtId="1" showAll="0"/>
-    <pivotField numFmtId="1" showAll="0"/>
-    <pivotField numFmtId="1" showAll="0"/>
-    <pivotField numFmtId="1" showAll="0"/>
-    <pivotField numFmtId="1" showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField dataField="1" numFmtId="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="50">
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="39"/>
-    </i>
-    <i>
-      <x v="46"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="41"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="45"/>
-    </i>
-    <i>
-      <x v="43"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="47"/>
-    </i>
-    <i>
-      <x v="48"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Suma de Suma de todos los Servicios" fld="11" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F2231237-FEAB-409D-B0B0-7D68E8795616}" name="TablaDinámica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="21">
   <location ref="A7:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
@@ -36427,7 +37779,7 @@
   <dataFields count="1">
     <dataField name="Suma de Total de cada servicio" fld="1" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
-  <chartFormats count="10">
+  <chartFormats count="18">
     <chartFormat chart="6" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -36531,6 +37883,102 @@
       </pivotArea>
     </chartFormat>
     <chartFormat chart="14" format="18">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="8">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -58190,7 +59638,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -58205,7 +59653,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
refactor: Se mejoralo el gráfico de línea de tiempo
</commit_message>
<xml_diff>
--- a/Dashboard/Dashboard.xlsx
+++ b/Dashboard/Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\servicios_cul_soci_depor_recre\Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF6A3BD-4969-4520-98CC-E729C3505218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA0B8F1-6CE9-4DC1-8609-74A79523A023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" firstSheet="1" activeTab="6" xr2:uid="{0F6DE12B-782F-43E4-BCEE-D62EF1718F31}"/>
   </bookViews>
@@ -940,9 +940,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00B4D8"/>
+      <color rgb="FF0077B6"/>
       <color rgb="FF90E0EF"/>
       <color rgb="FF03045E"/>
-      <color rgb="FF0077B6"/>
       <color rgb="FFCAF0F8"/>
     </mruColors>
   </colors>
@@ -11147,7 +11148,7 @@
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="0077B6"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -11158,7 +11159,7 @@
           <c:size val="5"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="00B4D8"/>
             </a:solidFill>
             <a:ln w="9525">
               <a:solidFill>
@@ -11184,16 +11185,16 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="75000"/>
                       <a:lumOff val="25000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="es-MX"/>
@@ -13058,7 +13059,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="0077B6"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -13069,7 +13070,7 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="00B4D8"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
@@ -13094,16 +13095,16 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
                         <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="es-MX"/>
@@ -13282,16 +13283,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="es-MX"/>
@@ -13315,9 +13316,8 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -13341,16 +13341,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="es-MX"/>
@@ -13368,37 +13368,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="0"/>
@@ -13411,16 +13380,9 @@
     </c:extLst>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -24802,16 +24764,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>569594</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>655320</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>81915</xdr:rowOff>
+      <xdr:rowOff>5714</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>158115</xdr:rowOff>
+      <xdr:rowOff>175259</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -35794,7 +35756,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1F62BD48-AAC3-4695-8D01-0E115DAB1328}" name="ServiciosDeportivosPorAño" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Años" colHeaderCaption="Nombre Oficina Representación">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1F62BD48-AAC3-4695-8D01-0E115DAB1328}" name="ServiciosDeportivosPorAño" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10" rowHeaderCaption="Años" colHeaderCaption="Nombre Oficina Representación">
   <location ref="A6:B21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" numFmtId="1" showAll="0">
@@ -37135,7 +37097,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{925D5B79-7889-4349-AA7F-C5C2592F1090}" name="ComparaciónEntreServiciosCulturalesVsDeportivosVsSociales" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14" rowHeaderCaption="Nombre Oficina Representación">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{925D5B79-7889-4349-AA7F-C5C2592F1090}" name="ComparaciónEntreServiciosCulturalesVsDeportivosVsSociales" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15" rowHeaderCaption="Nombre Oficina Representación">
   <location ref="A6:I7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField numFmtId="1" showAll="0">
@@ -66524,7 +66486,7 @@
   <dimension ref="A1:AR88"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
refactor: Se edito el gráfico de barras Top 10
</commit_message>
<xml_diff>
--- a/Dashboard/Dashboard.xlsx
+++ b/Dashboard/Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\servicios_cul_soci_depor_recre\Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA0B8F1-6CE9-4DC1-8609-74A79523A023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBC6CE1-6627-48F2-B58F-2AEE7D080E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" firstSheet="1" activeTab="6" xr2:uid="{0F6DE12B-782F-43E4-BCEE-D62EF1718F31}"/>
   </bookViews>
@@ -940,11 +940,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCAF0F8"/>
+      <color rgb="FF03045E"/>
+      <color rgb="FF0077B6"/>
       <color rgb="FF00B4D8"/>
-      <color rgb="FF0077B6"/>
       <color rgb="FF90E0EF"/>
-      <color rgb="FF03045E"/>
-      <color rgb="FFCAF0F8"/>
     </mruColors>
   </colors>
   <extLst>
@@ -11187,10 +11187,7 @@
               <a:pPr>
                 <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
@@ -13097,10 +13094,7 @@
                 <a:pPr>
                   <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
@@ -13285,10 +13279,7 @@
             <a:pPr>
               <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
@@ -13343,10 +13334,7 @@
             <a:pPr>
               <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
@@ -16307,16 +16295,13 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="es-MX"/>
@@ -16446,7 +16431,7 @@
         <c:idx val="32"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent1"/>
+            <a:srgbClr val="CAF0F8"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -16668,9 +16653,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="80000"/>
-                </a:schemeClr>
+                <a:srgbClr val="CAF0F8"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -16698,16 +16681,13 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="es-MX"/>
@@ -16866,16 +16846,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="es-MX"/>
@@ -16923,16 +16900,9 @@
     </c:extLst>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -24841,15 +24811,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
+      <xdr:colOff>579120</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>81915</xdr:rowOff>
+      <xdr:rowOff>120015</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>150495</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -37650,7 +37620,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{97A441A6-56C0-4FFA-911D-41686AFDD066}" name="RankingDeDelegaciones" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11" rowHeaderCaption="Nombre Oficina Representación">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{97A441A6-56C0-4FFA-911D-41686AFDD066}" name="RankingDeDelegaciones" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12" rowHeaderCaption="Nombre Oficina Representación">
   <location ref="A9:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField numFmtId="1" showAll="0">
@@ -66486,7 +66456,7 @@
   <dimension ref="A1:AR88"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
refactor: Mejora al estilo de los segmentadores de datos
</commit_message>
<xml_diff>
--- a/Dashboard/Dashboard.xlsx
+++ b/Dashboard/Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\servicios_cul_soci_depor_recre\Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7372C4-4BB0-43DA-A8E6-766A0E2F2F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBD7922-C91B-4223-8086-0B032F87C6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" firstSheet="2" activeTab="6" xr2:uid="{0F6DE12B-782F-43E4-BCEE-D62EF1718F31}"/>
   </bookViews>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -895,7 +895,45 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <sz val="11"/>
+        <name val="Arial Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0"/>
+          <bgColor rgb="FF90E0EF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF90E0EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -936,19 +974,152 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Estilo de segmentación de datos 1" pivot="0" table="0" count="1" xr9:uid="{04E74823-5D2C-400C-947C-9D106FE661C9}">
+      <tableStyleElement type="wholeTable" dxfId="3"/>
+    </tableStyle>
+    <tableStyle name="Estilo de segmentación de datos 2" pivot="0" table="0" count="1" xr9:uid="{9C4A7FAD-D90B-4111-B5BD-0AF484B2DE7C}">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+    </tableStyle>
+    <tableStyle name="Estilo de segmentación de datos 3" pivot="0" table="0" count="4" xr9:uid="{0139C86D-A396-4C00-87B8-19021044F397}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF0077B6"/>
+      <color rgb="FF90E0EF"/>
+      <color rgb="FF03045E"/>
       <color rgb="FFCAF0F8"/>
-      <color rgb="FF03045E"/>
-      <color rgb="FF0077B6"/>
       <color rgb="FF00B4D8"/>
-      <color rgb="FF90E0EF"/>
     </mruColors>
   </colors>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{46F421CA-312F-682f-3DD2-61675219B42D}">
+      <x14:dxfs count="14">
+        <dxf>
+          <border>
+            <left style="thin">
+              <color auto="1"/>
+            </left>
+            <right style="thin">
+              <color auto="1"/>
+            </right>
+            <top style="thin">
+              <color auto="1"/>
+            </top>
+            <bottom style="thin">
+              <color auto="1"/>
+            </bottom>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <b val="0"/>
+            <i val="0"/>
+            <sz val="11"/>
+            <color theme="0"/>
+            <name val="Arial"/>
+            <family val="2"/>
+            <scheme val="none"/>
+          </font>
+          <fill>
+            <patternFill>
+              <bgColor rgb="FF0077B6"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color auto="1"/>
+            </left>
+            <right style="thin">
+              <color auto="1"/>
+            </right>
+            <top style="thin">
+              <color auto="1"/>
+            </top>
+            <bottom style="thin">
+              <color auto="1"/>
+            </bottom>
+            <vertical style="thin">
+              <color auto="1"/>
+            </vertical>
+            <horizontal style="thin">
+              <color auto="1"/>
+            </horizontal>
+          </border>
+        </dxf>
+        <dxf/>
+        <dxf>
+          <font>
+            <b val="0"/>
+            <i val="0"/>
+            <sz val="11"/>
+            <color theme="0"/>
+            <name val="Arial"/>
+            <family val="2"/>
+            <scheme val="none"/>
+          </font>
+          <fill>
+            <patternFill>
+              <bgColor rgb="FF0077B6"/>
+            </patternFill>
+          </fill>
+        </dxf>
+        <dxf/>
+        <dxf>
+          <font>
+            <b val="0"/>
+            <i val="0"/>
+            <sz val="11"/>
+            <color theme="0"/>
+            <name val="Arial"/>
+            <family val="2"/>
+            <scheme val="none"/>
+          </font>
+          <fill>
+            <patternFill>
+              <bgColor rgb="FF0077B6"/>
+            </patternFill>
+          </fill>
+        </dxf>
+        <dxf/>
+        <dxf>
+          <font>
+            <color theme="0"/>
+          </font>
+          <fill>
+            <patternFill>
+              <bgColor rgb="FF0077B6"/>
+            </patternFill>
+          </fill>
+        </dxf>
+        <dxf>
+          <fill>
+            <patternFill>
+              <bgColor rgb="FF0077B6"/>
+            </patternFill>
+          </fill>
+        </dxf>
+        <dxf/>
+        <dxf/>
+        <dxf/>
+        <dxf/>
+        <dxf/>
+      </x14:dxfs>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1">
+        <x14:slicerStyle name="Estilo de segmentación de datos 1"/>
+        <x14:slicerStyle name="Estilo de segmentación de datos 2"/>
+        <x14:slicerStyle name="Estilo de segmentación de datos 3">
+          <x14:slicerStyleElements>
+            <x14:slicerStyleElement type="selectedItemWithData" dxfId="1"/>
+            <x14:slicerStyleElement type="selectedItemWithNoData" dxfId="0"/>
+          </x14:slicerStyleElements>
+        </x14:slicerStyle>
+      </x14:slicerStyles>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
@@ -24511,13 +24682,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>33867</xdr:rowOff>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>8466</xdr:colOff>
+      <xdr:colOff>214206</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
@@ -24534,8 +24705,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="1131147"/>
-          <a:ext cx="2385906" cy="6161193"/>
+          <a:off x="205740" y="1684020"/>
+          <a:ext cx="2385906" cy="5608320"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -24544,8 +24715,17 @@
           <a:srgbClr val="90E0EF"/>
         </a:solidFill>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:srgbClr val="03045E"/>
+          </a:solidFill>
         </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -26374,18 +26554,18 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>158115</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="33" name="Oficina Representación">
@@ -26408,7 +26588,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -26418,8 +26598,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="220980" y="1348740"/>
-              <a:ext cx="1828800" cy="2466975"/>
+              <a:off x="289560" y="1836420"/>
+              <a:ext cx="2217420" cy="3154680"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -26452,18 +26632,18 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>68581</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="34" name="Año">
@@ -26486,7 +26666,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -26496,8 +26676,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="274320" y="3931920"/>
-              <a:ext cx="1828800" cy="2466975"/>
+              <a:off x="396240" y="5006341"/>
+              <a:ext cx="2004060" cy="2217419"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -40951,8 +41131,8 @@
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
-  <slicer name="Oficina Representación" xr10:uid="{0C780604-6BF9-43A0-ABB5-6ACF2D70C2C7}" cache="SegmentaciónDeDatos_Oficina_Representación" caption="Oficina Representación" startItem="13" rowHeight="234950"/>
-  <slicer name="Año" xr10:uid="{0E312A47-3608-45BD-9A90-F091450EC507}" cache="SegmentaciónDeDatos_Año" caption="Año" startItem="5" rowHeight="234950"/>
+  <slicer name="Oficina Representación" xr10:uid="{0C780604-6BF9-43A0-ABB5-6ACF2D70C2C7}" cache="SegmentaciónDeDatos_Oficina_Representación" caption="Oficina Representación" startItem="8" columnCount="2" style="Estilo de segmentación de datos 3" rowHeight="234950"/>
+  <slicer name="Año" xr10:uid="{0E312A47-3608-45BD-9A90-F091450EC507}" cache="SegmentaciónDeDatos_Año" caption="Año" startItem="2" columnCount="2" style="Estilo de segmentación de datos 3" rowHeight="234950"/>
 </slicers>
 </file>
 
@@ -40963,18 +41143,18 @@
     <sortCondition descending="1" ref="L1:L495"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{E00903E2-5B95-4A2E-B89D-5B0052D7F544}" name="Año" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{E00903E2-5B95-4A2E-B89D-5B0052D7F544}" name="Año" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{6015B546-CCE8-49F7-AD82-A56721BEB06D}" name="Oficina Representación"/>
-    <tableColumn id="3" xr3:uid="{6C24FA5D-647C-4DF8-A6EA-66A6E6528CE5}" name="Serv. Culturales Derecho Hab Publ" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{5625FA80-061B-464D-B123-C974C04DA294}" name="Serv. Deportivos Derecho Hab Publ" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{24DE0E05-24AF-4FCC-9633-B84A75B97D9A}" name="Serv. Sociales Derecho Hab Publ" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{2AC1C74A-7627-48C3-AC0B-15FBB8351EE0}" name="Serv. Funerarios Derecho Hab Publ" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{3E1E2BD6-8333-4561-B9F1-248EFBB7920E}" name="Serv. Sociales Pensionados Jubl" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{2AC1B96B-1C99-43AF-AFED-47F1F4C408FD}" name="Fome Deportivo Pensionados Jubl" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{E70B6682-15CA-4E92-BD60-818587E36A59}" name="Serv. Culturales Pensionados Jubl" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{08067B72-2814-4712-B380-BB03A667992C}" name="Soci Comedores Pensionados Jubl" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{230A8DA6-C4FF-44BE-9A39-A60006ECF43E}" name="Fecha" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{859920B6-B83D-4724-917B-E5C66D0C0364}" name="Suma de todos los Servicios" dataDxfId="2">
+    <tableColumn id="3" xr3:uid="{6C24FA5D-647C-4DF8-A6EA-66A6E6528CE5}" name="Serv. Culturales Derecho Hab Publ" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{5625FA80-061B-464D-B123-C974C04DA294}" name="Serv. Deportivos Derecho Hab Publ" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{24DE0E05-24AF-4FCC-9633-B84A75B97D9A}" name="Serv. Sociales Derecho Hab Publ" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{2AC1C74A-7627-48C3-AC0B-15FBB8351EE0}" name="Serv. Funerarios Derecho Hab Publ" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{3E1E2BD6-8333-4561-B9F1-248EFBB7920E}" name="Serv. Sociales Pensionados Jubl" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{2AC1B96B-1C99-43AF-AFED-47F1F4C408FD}" name="Fome Deportivo Pensionados Jubl" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{E70B6682-15CA-4E92-BD60-818587E36A59}" name="Serv. Culturales Pensionados Jubl" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{08067B72-2814-4712-B380-BB03A667992C}" name="Soci Comedores Pensionados Jubl" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{230A8DA6-C4FF-44BE-9A39-A60006ECF43E}" name="Fecha" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{859920B6-B83D-4724-917B-E5C66D0C0364}" name="Suma de todos los Servicios" dataDxfId="6">
       <calculatedColumnFormula>SUM(Tabla1[[#This Row],[Serv. Culturales Derecho Hab Publ]:[Soci Comedores Pensionados Jubl]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -40986,8 +41166,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{943BA7B8-89FD-4590-985A-D669DB928326}" name="Tabla3" displayName="Tabla3" ref="B505:C513" totalsRowShown="0">
   <autoFilter ref="B505:C513" xr:uid="{943BA7B8-89FD-4590-985A-D669DB928326}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{52308A83-3E58-4597-85E5-390E9550E560}" name="Nombre Servicio" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{DDDD0592-6492-4A2A-BC52-9B55A82E2E0F}" name="Total de cada servicio" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{52308A83-3E58-4597-85E5-390E9550E560}" name="Nombre Servicio" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{DDDD0592-6492-4A2A-BC52-9B55A82E2E0F}" name="Total de cada servicio" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -66806,7 +66986,7 @@
   <dimension ref="A1:AR88"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feat: Presentación de la hoja como Dashboard
</commit_message>
<xml_diff>
--- a/Dashboard/Dashboard.xlsx
+++ b/Dashboard/Dashboard.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Data Scientist\Portafolio\servicios_cul_soci_depor_recre\Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBD7922-C91B-4223-8086-0B032F87C6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8198ECE-20DA-4B59-8207-0AA36F820FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" firstSheet="2" activeTab="6" xr2:uid="{0F6DE12B-782F-43E4-BCEE-D62EF1718F31}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="6" xr2:uid="{0F6DE12B-782F-43E4-BCEE-D62EF1718F31}"/>
   </bookViews>
   <sheets>
     <sheet name="servicios_cult_soc_dep_rec_isss" sheetId="1" r:id="rId1"/>
@@ -997,7 +997,7 @@
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{46F421CA-312F-682f-3DD2-61675219B42D}">
-      <x14:dxfs count="14">
+      <x14:dxfs count="2">
         <dxf>
           <border>
             <left style="thin">
@@ -1050,63 +1050,6 @@
             </horizontal>
           </border>
         </dxf>
-        <dxf/>
-        <dxf>
-          <font>
-            <b val="0"/>
-            <i val="0"/>
-            <sz val="11"/>
-            <color theme="0"/>
-            <name val="Arial"/>
-            <family val="2"/>
-            <scheme val="none"/>
-          </font>
-          <fill>
-            <patternFill>
-              <bgColor rgb="FF0077B6"/>
-            </patternFill>
-          </fill>
-        </dxf>
-        <dxf/>
-        <dxf>
-          <font>
-            <b val="0"/>
-            <i val="0"/>
-            <sz val="11"/>
-            <color theme="0"/>
-            <name val="Arial"/>
-            <family val="2"/>
-            <scheme val="none"/>
-          </font>
-          <fill>
-            <patternFill>
-              <bgColor rgb="FF0077B6"/>
-            </patternFill>
-          </fill>
-        </dxf>
-        <dxf/>
-        <dxf>
-          <font>
-            <color theme="0"/>
-          </font>
-          <fill>
-            <patternFill>
-              <bgColor rgb="FF0077B6"/>
-            </patternFill>
-          </fill>
-        </dxf>
-        <dxf>
-          <fill>
-            <patternFill>
-              <bgColor rgb="FF0077B6"/>
-            </patternFill>
-          </fill>
-        </dxf>
-        <dxf/>
-        <dxf/>
-        <dxf/>
-        <dxf/>
-        <dxf/>
       </x14:dxfs>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -4495,7 +4438,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4578,43 +4521,43 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>79355</c:v>
+                  <c:v>63099</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>70442</c:v>
+                  <c:v>63296</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71296</c:v>
+                  <c:v>64023</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>72504</c:v>
+                  <c:v>44394</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72045</c:v>
+                  <c:v>46664</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72759</c:v>
+                  <c:v>39688</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15133</c:v>
+                  <c:v>5275</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>884</c:v>
+                  <c:v>521</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>626</c:v>
+                  <c:v>719</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>638</c:v>
+                  <c:v>540</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>756</c:v>
+                  <c:v>440</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>252</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5425,7 +5368,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5437,7 +5380,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>840418</c:v>
+                  <c:v>37452</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5536,7 +5479,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5548,7 +5491,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>456690</c:v>
+                  <c:v>46664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5647,7 +5590,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5659,7 +5602,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>239</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5758,7 +5701,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5770,7 +5713,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1038</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5869,7 +5812,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5881,7 +5824,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>22652</c:v>
+                  <c:v>4111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5980,7 +5923,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5992,7 +5935,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>19799</c:v>
+                  <c:v>3037</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6093,7 +6036,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6105,7 +6048,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>55410</c:v>
+                  <c:v>18098</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6206,7 +6149,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6937,31 +6880,31 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Nuevo León</c:v>
+                  <c:v>Coahuila</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Coahuila</c:v>
+                  <c:v>Hidalgo</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Delegación Sur</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Yucatán</c:v>
+                  <c:v>Zacatecas</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Zacatecas</c:v>
+                  <c:v>Delegación Norte</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>México</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>Delegación Poniente</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>San Luis Potosí</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Oaxaca</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Áreas Centrales</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Oficinas Centrales</c:v>
@@ -6976,34 +6919,34 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1151362</c:v>
+                  <c:v>223652</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1329318</c:v>
+                  <c:v>225894</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1396246</c:v>
+                  <c:v>236430</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1544155</c:v>
+                  <c:v>256818</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1700361</c:v>
+                  <c:v>289376</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1853200</c:v>
+                  <c:v>298452</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2141268</c:v>
+                  <c:v>313541</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2824608</c:v>
+                  <c:v>316814</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2908515</c:v>
+                  <c:v>459232</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12806883</c:v>
+                  <c:v>1888180</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13218,7 +13161,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -13356,43 +13299,43 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>79355</c:v>
+                  <c:v>63099</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>70442</c:v>
+                  <c:v>63296</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71296</c:v>
+                  <c:v>64023</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>72504</c:v>
+                  <c:v>44394</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72045</c:v>
+                  <c:v>46664</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72759</c:v>
+                  <c:v>39688</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15133</c:v>
+                  <c:v>5275</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>884</c:v>
+                  <c:v>521</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>626</c:v>
+                  <c:v>719</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>638</c:v>
+                  <c:v>540</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>756</c:v>
+                  <c:v>440</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>252</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15073,7 +15016,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -15085,7 +15028,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>840418</c:v>
+                  <c:v>37452</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15184,7 +15127,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -15196,7 +15139,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>456690</c:v>
+                  <c:v>46664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15295,7 +15238,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -15307,7 +15250,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>239</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15408,7 +15351,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -15420,7 +15363,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1038</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15521,7 +15464,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -15533,7 +15476,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>22652</c:v>
+                  <c:v>4111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15634,7 +15577,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -15646,7 +15589,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>19799</c:v>
+                  <c:v>3037</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15748,7 +15691,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -15760,7 +15703,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>55410</c:v>
+                  <c:v>18098</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15862,7 +15805,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Guanajuato</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -16891,31 +16834,31 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Nuevo León</c:v>
+                  <c:v>Coahuila</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Coahuila</c:v>
+                  <c:v>Hidalgo</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Hidalgo</c:v>
+                  <c:v>Delegación Sur</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Yucatán</c:v>
+                  <c:v>Zacatecas</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Zacatecas</c:v>
+                  <c:v>Delegación Norte</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>México</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>Delegación Poniente</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>San Luis Potosí</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Oaxaca</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Áreas Centrales</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Oficinas Centrales</c:v>
@@ -16930,34 +16873,34 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1151362</c:v>
+                  <c:v>223652</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1329318</c:v>
+                  <c:v>225894</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1396246</c:v>
+                  <c:v>236430</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1544155</c:v>
+                  <c:v>256818</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1700361</c:v>
+                  <c:v>289376</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1853200</c:v>
+                  <c:v>298452</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2141268</c:v>
+                  <c:v>313541</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2824608</c:v>
+                  <c:v>316814</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2908515</c:v>
+                  <c:v>459232</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12806883</c:v>
+                  <c:v>1888180</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -24052,7 +23995,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t>12806883</a:t>
+            <a:t>1888180</a:t>
           </a:fld>
           <a:endParaRPr lang="es-MX" sz="1400" b="1">
             <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
@@ -25759,7 +25702,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t>12806883</a:t>
+            <a:t>1888180</a:t>
           </a:fld>
           <a:endParaRPr lang="es-MX" sz="1200" b="1">
             <a:solidFill>
@@ -26554,15 +26497,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
+      <xdr:colOff>281940</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
+      <xdr:colOff>121920</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -26575,7 +26518,9 @@
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
+            <xdr:cNvGraphicFramePr>
+              <a:graphicFrameLocks noMove="1" noResize="1"/>
+            </xdr:cNvGraphicFramePr>
           </xdr:nvGraphicFramePr>
           <xdr:xfrm>
             <a:off x="0" y="0"/>
@@ -26598,8 +26543,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="289560" y="1836420"/>
-              <a:ext cx="2217420" cy="3154680"/>
+              <a:off x="281940" y="1831041"/>
+              <a:ext cx="2206662" cy="3093720"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -26627,7 +26572,7 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
-    <xdr:clientData/>
+    <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -26653,7 +26598,9 @@
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
+            <xdr:cNvGraphicFramePr>
+              <a:graphicFrameLocks noMove="1" noResize="1"/>
+            </xdr:cNvGraphicFramePr>
           </xdr:nvGraphicFramePr>
           <xdr:xfrm>
             <a:off x="0" y="0"/>
@@ -26676,8 +26623,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="396240" y="5006341"/>
-              <a:ext cx="2004060" cy="2217419"/>
+              <a:off x="396240" y="4909522"/>
+              <a:ext cx="1993302" cy="2174389"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -26705,7 +26652,7 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
-    <xdr:clientData/>
+    <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -36314,9 +36261,9 @@
         <item h="1" x="48"/>
         <item h="1" x="46"/>
         <item h="1" x="8"/>
-        <item h="1" x="9"/>
+        <item x="9"/>
         <item h="1" x="10"/>
-        <item x="11"/>
+        <item h="1" x="11"/>
         <item h="1" x="37"/>
         <item h="1" x="12"/>
         <item h="1" x="13"/>
@@ -36412,7 +36359,7 @@
   </colFields>
   <colItems count="1">
     <i>
-      <x v="19"/>
+      <x v="17"/>
     </i>
   </colItems>
   <dataFields count="1">
@@ -37620,19 +37567,19 @@
   <pivotFields count="12">
     <pivotField numFmtId="1" showAll="0">
       <items count="14">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item h="1" x="4"/>
         <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
+        <item h="1" x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="8"/>
+        <item h="1" x="9"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item h="1" x="12"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -37655,9 +37602,9 @@
         <item h="1" x="48"/>
         <item h="1" x="46"/>
         <item h="1" x="8"/>
-        <item h="1" x="9"/>
+        <item x="9"/>
         <item h="1" x="10"/>
-        <item x="11"/>
+        <item h="1" x="11"/>
         <item h="1" x="37"/>
         <item h="1" x="12"/>
         <item h="1" x="13"/>
@@ -37706,7 +37653,7 @@
   </rowFields>
   <rowItems count="1">
     <i>
-      <x v="19"/>
+      <x v="17"/>
     </i>
   </rowItems>
   <colFields count="1">
@@ -37921,19 +37868,19 @@
   <pivotFields count="12">
     <pivotField numFmtId="1" showAll="0">
       <items count="14">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item h="1" x="4"/>
         <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
+        <item h="1" x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="8"/>
+        <item h="1" x="9"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item h="1" x="12"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -40175,31 +40122,31 @@
   </rowFields>
   <rowItems count="11">
     <i>
-      <x v="26"/>
-    </i>
-    <i>
       <x v="8"/>
     </i>
     <i>
       <x v="19"/>
     </i>
     <i>
-      <x v="47"/>
+      <x v="15"/>
     </i>
     <i>
       <x v="48"/>
     </i>
     <i>
+      <x v="12"/>
+    </i>
+    <i>
       <x v="22"/>
+    </i>
+    <i>
+      <x v="14"/>
     </i>
     <i>
       <x v="36"/>
     </i>
     <i>
       <x v="27"/>
-    </i>
-    <i>
-      <x v="1"/>
     </i>
     <i>
       <x v="28"/>
@@ -41063,9 +41010,9 @@
         <i x="48"/>
         <i x="46"/>
         <i x="8"/>
-        <i x="9"/>
+        <i x="9" s="1"/>
         <i x="10"/>
-        <i x="11" s="1"/>
+        <i x="11"/>
         <i x="37"/>
         <i x="12"/>
         <i x="13"/>
@@ -41110,19 +41057,19 @@
   <data>
     <tabular pivotCacheId="747248475">
       <items count="13">
-        <i x="0" s="1"/>
-        <i x="1" s="1"/>
-        <i x="2" s="1"/>
-        <i x="3" s="1"/>
-        <i x="4" s="1"/>
+        <i x="0"/>
+        <i x="1"/>
+        <i x="2"/>
+        <i x="3"/>
+        <i x="4"/>
         <i x="5" s="1"/>
-        <i x="6" s="1"/>
-        <i x="7" s="1"/>
-        <i x="8" s="1"/>
-        <i x="9" s="1"/>
-        <i x="10" s="1"/>
-        <i x="11" s="1"/>
-        <i x="12" s="1"/>
+        <i x="6"/>
+        <i x="7"/>
+        <i x="8"/>
+        <i x="9"/>
+        <i x="10"/>
+        <i x="11"/>
+        <i x="12"/>
       </items>
     </tabular>
   </data>
@@ -41131,8 +41078,8 @@
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
-  <slicer name="Oficina Representación" xr10:uid="{0C780604-6BF9-43A0-ABB5-6ACF2D70C2C7}" cache="SegmentaciónDeDatos_Oficina_Representación" caption="Oficina Representación" startItem="8" columnCount="2" style="Estilo de segmentación de datos 3" rowHeight="234950"/>
-  <slicer name="Año" xr10:uid="{0E312A47-3608-45BD-9A90-F091450EC507}" cache="SegmentaciónDeDatos_Año" caption="Año" startItem="2" columnCount="2" style="Estilo de segmentación de datos 3" rowHeight="234950"/>
+  <slicer name="Oficina Representación" xr10:uid="{0C780604-6BF9-43A0-ABB5-6ACF2D70C2C7}" cache="SegmentaciónDeDatos_Oficina_Representación" caption="Oficina Representación" columnCount="2" style="Estilo de segmentación de datos 3" lockedPosition="1" rowHeight="234950"/>
+  <slicer name="Año" xr10:uid="{0E312A47-3608-45BD-9A90-F091450EC507}" cache="SegmentaciónDeDatos_Año" caption="Año" columnCount="2" style="Estilo de segmentación de datos 3" lockedPosition="1" rowHeight="234950"/>
 </slicers>
 </file>
 
@@ -41470,6 +41417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F449743-C6BA-4379-8C03-655115C7A180}">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:SE538"/>
   <sheetViews>
     <sheetView topLeftCell="A486" workbookViewId="0">
@@ -65513,6 +65461,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56573DCE-1102-4670-B2C5-59B84C64109B}">
+  <sheetPr codeName="Hoja2"/>
   <dimension ref="A2:F25"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
@@ -65594,7 +65543,7 @@
         <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -65602,7 +65551,7 @@
         <v>2013</v>
       </c>
       <c r="B8" s="2">
-        <v>79355</v>
+        <v>63099</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -65610,7 +65559,7 @@
         <v>2014</v>
       </c>
       <c r="B9" s="2">
-        <v>70442</v>
+        <v>63296</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -65618,7 +65567,7 @@
         <v>2015</v>
       </c>
       <c r="B10" s="2">
-        <v>71296</v>
+        <v>64023</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -65634,7 +65583,7 @@
         <v>2017</v>
       </c>
       <c r="B12" s="2">
-        <v>72504</v>
+        <v>44394</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -65642,7 +65591,7 @@
         <v>2018</v>
       </c>
       <c r="B13" s="2">
-        <v>72045</v>
+        <v>46664</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -65650,7 +65599,7 @@
         <v>2019</v>
       </c>
       <c r="B14" s="2">
-        <v>72759</v>
+        <v>39688</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -65658,7 +65607,7 @@
         <v>2020</v>
       </c>
       <c r="B15" s="2">
-        <v>15133</v>
+        <v>5275</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -65666,7 +65615,7 @@
         <v>2021</v>
       </c>
       <c r="B16" s="2">
-        <v>884</v>
+        <v>521</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -65674,7 +65623,7 @@
         <v>2022</v>
       </c>
       <c r="B17" s="2">
-        <v>626</v>
+        <v>719</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -65682,7 +65631,7 @@
         <v>2023</v>
       </c>
       <c r="B18" s="2">
-        <v>638</v>
+        <v>540</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -65690,7 +65639,7 @@
         <v>2024</v>
       </c>
       <c r="B19" s="2">
-        <v>756</v>
+        <v>440</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -65698,7 +65647,7 @@
         <v>2025</v>
       </c>
       <c r="B20" s="2">
-        <v>252</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -65706,7 +65655,7 @@
         <v>60</v>
       </c>
       <c r="B21" s="2">
-        <v>456690</v>
+        <v>328744</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="28.2" x14ac:dyDescent="0.5">
@@ -65730,6 +65679,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB971FC3-37E4-4473-BE72-831CFD6103DC}">
+  <sheetPr codeName="Hoja3"/>
   <dimension ref="A2:I60"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
@@ -65787,28 +65737,28 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
-        <v>840418</v>
+        <v>37452</v>
       </c>
       <c r="C7" s="2">
-        <v>456690</v>
+        <v>46664</v>
       </c>
       <c r="D7" s="2">
-        <v>239</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2">
-        <v>1038</v>
+        <v>108</v>
       </c>
       <c r="F7" s="2">
-        <v>22652</v>
+        <v>4111</v>
       </c>
       <c r="G7" s="2">
-        <v>19799</v>
+        <v>3037</v>
       </c>
       <c r="H7" s="2">
-        <v>55410</v>
+        <v>18098</v>
       </c>
       <c r="I7" s="2">
         <v>0</v>
@@ -65833,6 +65783,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803E057B-2FFD-452E-9801-D0EF6EE0D059}">
+  <sheetPr codeName="Hoja4"/>
   <dimension ref="A2:J83"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
@@ -66320,42 +66271,42 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2">
-        <v>1151362</v>
+        <v>223652</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>1329318</v>
+        <v>225894</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="B12" s="2">
-        <v>1396246</v>
+        <v>236430</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2">
-        <v>1544155</v>
+        <v>256818</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B14" s="2">
-        <v>1700361</v>
+        <v>289376</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -66363,31 +66314,31 @@
         <v>46</v>
       </c>
       <c r="B15" s="2">
-        <v>1853200</v>
+        <v>298452</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B16" s="2">
-        <v>2141268</v>
+        <v>313541</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B17" s="2">
-        <v>2824608</v>
+        <v>316814</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="B18" s="2">
-        <v>2908515</v>
+        <v>459232</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -66395,7 +66346,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="2">
-        <v>12806883</v>
+        <v>1888180</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -66403,7 +66354,7 @@
         <v>60</v>
       </c>
       <c r="B20" s="2">
-        <v>29655916</v>
+        <v>4508389</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -66418,7 +66369,7 @@
       </c>
       <c r="B28">
         <f ca="1">INDIRECT(B25)</f>
-        <v>12806883</v>
+        <v>1888180</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -66853,6 +66804,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEFD455-FE5D-4DB9-B672-24C684C812DC}">
+  <sheetPr codeName="Hoja5"/>
   <dimension ref="A7:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -66968,6 +66920,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E4A35B-1DEE-4E63-B176-45BEFEC88566}">
+  <sheetPr codeName="Hoja6"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -66983,11 +66936,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2626B9-BEDB-407F-B6C7-68E4D543C3D7}">
+  <sheetPr codeName="Hoja7"/>
   <dimension ref="A1:AR88"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
-    </sheetView>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -71040,6 +70992,7 @@
       <c r="AR88" s="10"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <extLst>

</xml_diff>